<commit_message>
added to inc_categories sheet, modified implementation of taxes in tax_incentives
</commit_message>
<xml_diff>
--- a/incentives/incentive_categories.xlsx
+++ b/incentives/incentive_categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/Biorefinery-Tax-Incentives/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4682A799-E515-4F4F-9A26-5E315DE2B4B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03A7B06-CF07-E345-8C8B-D89C84F5DB03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="660" windowWidth="23260" windowHeight="14020" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
+    <workbookView xWindow="4400" yWindow="3080" windowWidth="23260" windowHeight="14020" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="72">
   <si>
     <t>property</t>
   </si>
@@ -184,6 +184,63 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Variable type</t>
+  </si>
+  <si>
+    <t>value_added</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>property_taxable_value</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>biodiesel_eq</t>
+  </si>
+  <si>
+    <t>ethanol_eq</t>
+  </si>
+  <si>
+    <t>fuel_taxable_value</t>
+  </si>
+  <si>
+    <t>NM_value</t>
+  </si>
+  <si>
+    <t>wages</t>
+  </si>
+  <si>
+    <t>TCI</t>
+  </si>
+  <si>
+    <t>ethanol</t>
+  </si>
+  <si>
+    <t>state_income_tax_assessed</t>
+  </si>
+  <si>
+    <t>elec_eq</t>
+  </si>
+  <si>
+    <t>jobs_50</t>
+  </si>
+  <si>
+    <t>IA_value</t>
+  </si>
+  <si>
+    <t>building_mats</t>
+  </si>
+  <si>
+    <t>determine whether to pass integer or array</t>
   </si>
 </sst>
 </file>
@@ -596,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED89AE72-DC4E-BE45-96E4-63567237423A}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G24"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,11 +666,12 @@
     <col min="3" max="3" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="7" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -630,12 +688,18 @@
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -651,11 +715,17 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -671,10 +741,16 @@
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -690,10 +766,16 @@
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -709,10 +791,16 @@
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -728,9 +816,15 @@
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -746,9 +840,15 @@
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -764,12 +864,18 @@
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="3"/>
+      <c r="F8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="2"/>
       <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -785,12 +891,18 @@
       <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="3"/>
+      <c r="F9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="2"/>
       <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="3"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -806,9 +918,15 @@
       <c r="E10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -824,12 +942,18 @@
       <c r="E11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -845,10 +969,16 @@
       <c r="E12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -864,9 +994,15 @@
       <c r="E13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -882,10 +1018,16 @@
       <c r="E14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -901,11 +1043,17 @@
       <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -921,11 +1069,17 @@
       <c r="E16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -941,9 +1095,15 @@
       <c r="E17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -959,9 +1119,15 @@
       <c r="E18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -977,11 +1143,17 @@
       <c r="E19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="3"/>
+      <c r="F19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L19" s="3"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -997,11 +1169,17 @@
       <c r="E20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="3"/>
+      <c r="F20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="K20" s="8"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L20" s="3"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1017,10 +1195,16 @@
       <c r="E21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1036,10 +1220,16 @@
       <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1055,11 +1245,17 @@
       <c r="E23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="8"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1075,12 +1271,18 @@
       <c r="E24" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K24" s="6"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="3"/>
+      <c r="F24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M24" s="6"/>
       <c r="O24" s="8"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24" s="3"/>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>26</v>
       </c>
@@ -1096,23 +1298,23 @@
       <c r="E25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="N28" s="5"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K29" s="6"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="3"/>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M29" s="6"/>
       <c r="O29" s="8"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="N30" s="5"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="8"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="P30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added notes to incentives_TEA
</commit_message>
<xml_diff>
--- a/incentives/incentive_categories.xlsx
+++ b/incentives/incentive_categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/Biorefinery-Tax-Incentives/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03A7B06-CF07-E345-8C8B-D89C84F5DB03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C808BB4A-1240-A349-8022-D5D5EBE9485D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="3080" windowWidth="23260" windowHeight="14020" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
+    <workbookView xWindow="4400" yWindow="2280" windowWidth="23260" windowHeight="14020" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -656,7 +656,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixes to incentives_tea, changes to incentives_analysis, adding plots
</commit_message>
<xml_diff>
--- a/incentives/incentive_categories.xlsx
+++ b/incentives/incentive_categories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/Biorefinery-Tax-Incentives/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C808BB4A-1240-A349-8022-D5D5EBE9485D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB611BEF-951F-3549-9B14-6166D0357697}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4400" yWindow="2280" windowWidth="23260" windowHeight="14020" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
   </bookViews>
@@ -656,7 +656,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E2" sqref="E2:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates to analysis files
</commit_message>
<xml_diff>
--- a/incentives/incentive_categories.xlsx
+++ b/incentives/incentive_categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/Biorefinery-Tax-Incentives/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB611BEF-951F-3549-9B14-6166D0357697}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C02CC9F-C892-F84C-B138-CCC583044751}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="2280" windowWidth="23260" windowHeight="14020" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
+    <workbookView xWindow="2600" yWindow="920" windowWidth="23260" windowHeight="14020" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -304,21 +304,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -336,8 +327,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -656,7 +647,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E24"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1271,7 +1262,7 @@
       <c r="E24" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="9" t="s">
         <v>65</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -1284,23 +1275,31 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="F25" s="9"/>
       <c r="H25" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P28" s="5"/>

</xml_diff>